<commit_message>
Update Leave Card 4/18/2023 4:57 PM
</commit_message>
<xml_diff>
--- a/DOGELIO, CHRISTIAN.xlsx
+++ b/DOGELIO, CHRISTIAN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-44REB32\Users\ASUS\Desktop\LEAVECARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D432566D-8225-45F9-8CCF-61090E3E4056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -27,25 +28,17 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>PERIOD</t>
   </si>
@@ -271,11 +264,14 @@
   <si>
     <t>2023</t>
   </si>
+  <si>
+    <t>TOTAL LEAVE BALANCE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -651,9 +647,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -663,17 +656,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,27 +874,27 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
         <bottom style="thin">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -1119,27 +1115,27 @@
     <dxf>
       <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </left>
         <right style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </right>
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
@@ -1204,7 +1200,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1247,7 +1243,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1311,7 +1307,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1371,7 +1367,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1437,7 +1433,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1500,7 +1496,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1598,7 +1594,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1657,7 +1653,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1722,7 +1718,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1765,7 +1761,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1840,7 +1836,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2026,7 +2022,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2092,7 +2088,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2150,7 +2146,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2216,7 +2212,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2272,7 +2268,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2347,7 +2343,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2390,7 +2386,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2456,7 +2452,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2512,7 +2508,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2608,25 +2604,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K128" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K128" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2638,25 +2634,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K78" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K78" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2963,7 +2959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2973,7 +2969,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2981,97 +2977,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A64" activePane="bottomLeft"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3696" topLeftCell="A64" activePane="bottomLeft"/>
       <selection activeCell="I10" sqref="I10"/>
       <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="55">
         <v>42583</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -3079,7 +3075,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -3092,24 +3088,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -3144,7 +3140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -3168,7 +3164,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -3190,7 +3186,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -3210,7 +3206,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="49"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -3230,7 +3226,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -3250,7 +3246,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -3270,7 +3266,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -3290,7 +3286,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43252</v>
       </c>
@@ -3310,7 +3306,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -3330,7 +3326,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43313</v>
       </c>
@@ -3350,7 +3346,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43344</v>
       </c>
@@ -3370,7 +3366,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -3390,7 +3386,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -3410,7 +3406,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -3434,7 +3430,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>47</v>
       </c>
@@ -3452,7 +3448,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -3472,7 +3468,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -3492,7 +3488,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -3512,7 +3508,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -3532,7 +3528,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -3552,7 +3548,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -3572,7 +3568,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -3592,7 +3588,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -3616,7 +3612,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -3636,7 +3632,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -3662,7 +3658,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -3682,7 +3678,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -3702,7 +3698,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>57</v>
       </c>
@@ -3720,7 +3716,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -3740,7 +3736,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -3760,7 +3756,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -3780,7 +3776,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -3800,7 +3796,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -3820,7 +3816,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -3840,7 +3836,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -3860,7 +3856,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -3880,7 +3876,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -3900,7 +3896,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -3920,7 +3916,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -3940,7 +3936,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -3964,7 +3960,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>60</v>
       </c>
@@ -3982,7 +3978,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -4002,7 +3998,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -4022,7 +4018,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -4042,7 +4038,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -4062,7 +4058,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -4082,7 +4078,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -4102,7 +4098,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -4122,7 +4118,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -4142,7 +4138,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -4162,7 +4158,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -4182,7 +4178,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -4202,7 +4198,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -4226,7 +4222,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="48" t="s">
         <v>61</v>
       </c>
@@ -4244,7 +4240,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -4264,7 +4260,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -4284,7 +4280,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -4304,7 +4300,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40">
         <v>44652</v>
       </c>
@@ -4330,7 +4326,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44682</v>
       </c>
@@ -4350,7 +4346,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="49"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44713</v>
       </c>
@@ -4376,7 +4372,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40">
         <v>44743</v>
       </c>
@@ -4402,7 +4398,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40">
         <v>44774</v>
       </c>
@@ -4422,7 +4418,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44805</v>
       </c>
@@ -4448,7 +4444,7 @@
         <v>44824</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40">
         <v>44835</v>
       </c>
@@ -4468,7 +4464,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
         <v>44866</v>
       </c>
@@ -4494,7 +4490,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44896</v>
       </c>
@@ -4514,7 +4510,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="48" t="s">
         <v>74</v>
       </c>
@@ -4532,7 +4528,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40">
         <v>44927</v>
       </c>
@@ -4558,7 +4554,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -4574,7 +4570,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20"/>
       <c r="C78" s="13"/>
@@ -4590,7 +4586,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40"/>
       <c r="B79" s="20"/>
       <c r="C79" s="13"/>
@@ -4606,7 +4602,7 @@
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20"/>
       <c r="C80" s="13"/>
@@ -4622,7 +4618,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40"/>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
@@ -4638,7 +4634,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4654,7 +4650,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4670,7 +4666,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4686,7 +4682,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="23"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4702,7 +4698,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="23" t="s">
         <v>32</v>
       </c>
@@ -4720,7 +4716,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4736,7 +4732,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4752,7 +4748,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4768,7 +4764,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4784,7 +4780,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4800,7 +4796,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4816,7 +4812,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4832,7 +4828,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4848,7 +4844,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4864,7 +4860,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4880,7 +4876,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4896,7 +4892,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4912,7 +4908,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4928,7 +4924,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4944,7 +4940,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4960,7 +4956,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4976,7 +4972,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4992,7 +4988,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -5008,7 +5004,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -5024,7 +5020,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -5040,7 +5036,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -5056,7 +5052,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -5072,7 +5068,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5088,7 +5084,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5104,7 +5100,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5120,7 +5116,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5136,7 +5132,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5152,7 +5148,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5168,7 +5164,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5184,7 +5180,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5200,7 +5196,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5216,7 +5212,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5232,7 +5228,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5248,7 +5244,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5264,7 +5260,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5280,7 +5276,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5296,7 +5292,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5312,7 +5308,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5328,7 +5324,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5344,7 +5340,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5360,7 +5356,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5376,7 +5372,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="41"/>
       <c r="B128" s="15"/>
       <c r="C128" s="42"/>
@@ -5394,23 +5390,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5433,97 +5429,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A7" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A7" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="51"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="55">
         <v>42583</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="55"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -5531,7 +5527,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -5544,24 +5540,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -5596,7 +5592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -5620,7 +5616,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -5642,7 +5638,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -5664,7 +5660,7 @@
         <v>43126</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -5688,7 +5684,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="48" t="s">
         <v>47</v>
       </c>
@@ -5706,7 +5702,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43525</v>
       </c>
@@ -5728,7 +5724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43556</v>
       </c>
@@ -5752,7 +5748,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43739</v>
       </c>
@@ -5776,7 +5772,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="20" t="s">
         <v>55</v>
@@ -5798,7 +5794,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="48" t="s">
         <v>57</v>
       </c>
@@ -5816,7 +5812,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <v>43862</v>
       </c>
@@ -5838,7 +5834,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="48" t="s">
         <v>61</v>
       </c>
@@ -5856,7 +5852,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>44682</v>
       </c>
@@ -5880,7 +5876,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>44713</v>
       </c>
@@ -5904,7 +5900,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>44805</v>
       </c>
@@ -5926,7 +5922,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40"/>
       <c r="B24" s="20" t="s">
         <v>72</v>
@@ -5948,7 +5944,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="48" t="s">
         <v>74</v>
       </c>
@@ -5966,7 +5962,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>44927</v>
       </c>
@@ -5990,7 +5986,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40"/>
       <c r="B27" s="20"/>
       <c r="C27" s="13"/>
@@ -6006,7 +6002,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="20"/>
       <c r="C28" s="13"/>
@@ -6022,7 +6018,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="20"/>
       <c r="C29" s="13"/>
@@ -6038,7 +6034,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40"/>
       <c r="B30" s="20"/>
       <c r="C30" s="13"/>
@@ -6054,7 +6050,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="20"/>
       <c r="C31" s="13"/>
@@ -6070,7 +6066,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40"/>
       <c r="B32" s="20"/>
       <c r="C32" s="13"/>
@@ -6086,7 +6082,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40"/>
       <c r="B33" s="20"/>
       <c r="C33" s="13"/>
@@ -6102,7 +6098,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40"/>
       <c r="B34" s="20"/>
       <c r="C34" s="13"/>
@@ -6118,7 +6114,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="23"/>
       <c r="B35" s="20"/>
       <c r="C35" s="13"/>
@@ -6134,7 +6130,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="23" t="s">
         <v>32</v>
       </c>
@@ -6152,7 +6148,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -6168,7 +6164,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -6184,7 +6180,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -6200,7 +6196,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -6216,7 +6212,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -6232,7 +6228,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -6248,7 +6244,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -6264,7 +6260,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -6280,7 +6276,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -6296,7 +6292,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -6312,7 +6308,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -6328,7 +6324,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -6344,7 +6340,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -6360,7 +6356,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -6376,7 +6372,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -6392,7 +6388,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -6408,7 +6404,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -6424,7 +6420,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -6440,7 +6436,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -6456,7 +6452,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -6472,7 +6468,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -6488,7 +6484,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -6504,7 +6500,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -6520,7 +6516,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -6536,7 +6532,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -6552,7 +6548,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -6568,7 +6564,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -6584,7 +6580,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -6600,7 +6596,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -6616,7 +6612,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -6632,7 +6628,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -6648,7 +6644,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -6664,7 +6660,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -6680,7 +6676,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -6696,7 +6692,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -6712,7 +6708,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -6728,7 +6724,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -6744,7 +6740,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -6760,7 +6756,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40"/>
       <c r="B75" s="20"/>
       <c r="C75" s="13"/>
@@ -6776,7 +6772,7 @@
       <c r="J75" s="11"/>
       <c r="K75" s="20"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20"/>
       <c r="C76" s="13"/>
@@ -6792,7 +6788,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="20"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40"/>
       <c r="B77" s="20"/>
       <c r="C77" s="13"/>
@@ -6808,7 +6804,7 @@
       <c r="J77" s="11"/>
       <c r="K77" s="20"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="41"/>
       <c r="B78" s="15"/>
       <c r="C78" s="42"/>
@@ -6839,10 +6835,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6865,28 +6861,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -6899,7 +6895,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -6928,7 +6924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>10.75</v>
       </c>
@@ -6952,17 +6948,20 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -6983,7 +6982,11 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
+        <v>118.5</v>
+      </c>
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -7010,7 +7013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -7088,7 +7091,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -7114,7 +7117,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -7140,7 +7143,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -7166,7 +7169,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -7192,7 +7195,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -7212,7 +7215,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -7232,7 +7235,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -7252,7 +7255,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -7273,7 +7276,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -7294,7 +7297,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -7315,7 +7318,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -7336,7 +7339,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -7357,7 +7360,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -7399,7 +7402,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -7420,7 +7423,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -7441,7 +7444,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -7483,7 +7486,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -7504,7 +7507,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -7525,7 +7528,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -7546,7 +7549,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -7567,7 +7570,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -7588,7 +7591,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -7609,7 +7612,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -7630,7 +7633,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -7651,7 +7654,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -7672,7 +7675,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -7681,7 +7684,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -7690,7 +7693,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -7699,7 +7702,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -7708,7 +7711,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -7717,7 +7720,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -7726,7 +7729,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -7735,7 +7738,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -7744,7 +7747,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -7753,7 +7756,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -7762,7 +7765,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -7771,7 +7774,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -7780,7 +7783,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -7789,7 +7792,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -7798,7 +7801,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -7807,7 +7810,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -7816,7 +7819,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -7825,7 +7828,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -7834,7 +7837,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -7843,7 +7846,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -7852,7 +7855,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -7861,7 +7864,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -7870,7 +7873,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -7879,7 +7882,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -7888,7 +7891,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -7897,7 +7900,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -7906,7 +7909,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -7915,7 +7918,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -7924,7 +7927,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -7933,7 +7936,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>

<commit_message>
Update Leave Card 7/19/2023 4:27 PM
</commit_message>
<xml_diff>
--- a/DOGELIO, CHRISTIAN.xlsx
+++ b/DOGELIO, CHRISTIAN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>PERIOD</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>4/26,27,28/2023</t>
+  </si>
+  <si>
+    <t>7/7,12/2023</t>
   </si>
 </sst>
 </file>
@@ -655,14 +658,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -672,9 +678,6 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1205,7 +1208,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1251,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1312,7 +1315,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1375,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1438,7 +1441,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1504,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1599,7 +1602,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1658,7 +1661,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1723,7 +1726,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1766,7 +1769,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1841,7 +1844,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2027,7 +2030,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2093,7 +2096,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2151,7 +2154,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2217,7 +2220,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2273,7 +2276,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2348,7 +2351,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2391,7 +2394,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2457,7 +2460,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2513,7 +2516,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3021,14 +3024,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3039,16 +3042,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>42583</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3061,16 +3064,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3096,18 +3099,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5427,17 +5430,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -5475,7 +5478,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3690" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5505,14 +5508,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5523,16 +5526,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="55">
         <v>42583</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5545,16 +5548,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -5580,18 +5583,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5648,7 +5651,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>10.25</v>
+        <v>8.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -6049,7 +6052,9 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
-      <c r="B28" s="20"/>
+      <c r="B28" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="C28" s="13"/>
       <c r="D28" s="39"/>
       <c r="E28" s="9"/>
@@ -6058,10 +6063,14 @@
         <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
         <v/>
       </c>
-      <c r="H28" s="39"/>
+      <c r="H28" s="39">
+        <v>2</v>
+      </c>
       <c r="I28" s="9"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="20"/>
+      <c r="K28" s="20" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>

</xml_diff>